<commit_message>
add latest Rachel neut curves
</commit_message>
<xml_diff>
--- a/data/neut_plate_reader_data/HC060002.xlsx
+++ b/data/neut_plate_reader_data/HC060002.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/fh/fast/bloom_j/computational_notebooks/reguia/2020/validation/data/neut_plate_reader_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B13E22-864F-7647-A8AE-0428773DD993}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="21100" windowHeight="14860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F193D" sheetId="5" r:id="rId1"/>
     <sheet name="K189D" sheetId="4" r:id="rId2"/>
     <sheet name="F193F" sheetId="3" r:id="rId3"/>
     <sheet name="WT" sheetId="2" r:id="rId4"/>
+    <sheet name="I192E" sheetId="6" r:id="rId5"/>
+    <sheet name="F159G" sheetId="7" r:id="rId6"/>
+    <sheet name="WT2" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eguia, Rachel T</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -30,7 +39,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
 Tecan.At.Common.DocumentManagement, 3.3.10.0
@@ -84,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +101,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -108,12 +117,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eguia, Rachel T</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -121,7 +130,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
 Tecan.At.Common.DocumentManagement, 3.3.10.0
@@ -175,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +192,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -199,12 +208,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eguia, Rachel T</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +221,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
 Tecan.At.Common.DocumentManagement, 3.3.10.0
@@ -266,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -274,7 +283,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -290,12 +299,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eguia, Rachel T</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -303,7 +312,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
 Tecan.At.Common.DocumentManagement, 3.3.10.0
@@ -357,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -365,7 +374,280 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -381,7 +663,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="72">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -564,12 +846,45 @@
   </si>
   <si>
     <t>3/23/2020 7:57:38 AM</t>
+  </si>
+  <si>
+    <t>5/2/2020 9:42:45 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 23.2 °C</t>
+  </si>
+  <si>
+    <t>5/2/2020 9:41:49 AM</t>
+  </si>
+  <si>
+    <t>9:40:50 AM</t>
+  </si>
+  <si>
+    <t>5/2/2020 9:40:34 AM</t>
+  </si>
+  <si>
+    <t>5/2/2020 9:39:38 AM</t>
+  </si>
+  <si>
+    <t>9:38:35 AM</t>
+  </si>
+  <si>
+    <t>5/2/2020 9:38:19 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 22.9 °C</t>
+  </si>
+  <si>
+    <t>5/2/2020 9:37:24 AM</t>
+  </si>
+  <si>
+    <t>9:36:25 AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,10 +912,10 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -651,60 +966,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7FFFD4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6495ED"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF32CD32"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9ACD32"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8FBC8B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDEB887"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4A460"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD2691E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -733,23 +994,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6"/>
-    <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7"/>
-    <cellStyle name="Tecan.At.Excel.Error" xfId="1"/>
-    <cellStyle name="Tecan.At.Excel.GFactorAndMeasurementBlank" xfId="5"/>
-    <cellStyle name="Tecan.At.Excel.GFactorBlank" xfId="3"/>
-    <cellStyle name="Tecan.At.Excel.GFactorReference" xfId="4"/>
-    <cellStyle name="Tecan.At.Excel.MeasurementBlank" xfId="2"/>
+    <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Tecan.At.Excel.Error" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorAndMeasurementBlank" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorBlank" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Tecan.At.Excel.GFactorReference" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Tecan.At.Excel.MeasurementBlank" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -798,7 +1062,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -831,9 +1095,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -866,6 +1147,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1041,14 +1339,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1064,7 +1362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1072,7 +1370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1080,7 +1378,7 @@
         <v>43913</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1386,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1104,7 +1402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1112,17 +1410,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1130,12 +1428,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1146,7 +1444,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1157,7 +1455,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1168,7 +1466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1179,7 +1477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1488,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1212,7 +1510,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1223,7 +1521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1234,7 +1532,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1245,7 +1543,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1253,12 +1551,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1299,7 +1597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -1340,7 +1638,7 @@
         <v>8622</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -1381,7 +1679,7 @@
         <v>11530</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -1422,7 +1720,7 @@
         <v>30004</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -1463,7 +1761,7 @@
         <v>12725</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -1504,7 +1802,7 @@
         <v>12661</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -1545,7 +1843,7 @@
         <v>12427</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -1586,7 +1884,7 @@
         <v>28208</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -1627,7 +1925,7 @@
         <v>7889</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1642,14 +1940,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1665,7 +1963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1673,7 +1971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1681,7 +1979,7 @@
         <v>43913</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1689,7 +1987,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1697,7 +1995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1705,7 +2003,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1713,17 +2011,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1731,12 +2029,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1747,7 +2045,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1758,7 +2056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1769,7 +2067,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1780,7 +2078,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1791,7 +2089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1802,7 +2100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1813,7 +2111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1824,7 +2122,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1835,7 +2133,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1846,7 +2144,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1854,12 +2152,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1900,7 +2198,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -1941,7 +2239,7 @@
         <v>10774</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -1982,7 +2280,7 @@
         <v>13458</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -2023,7 +2321,7 @@
         <v>38935</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -2064,7 +2362,7 @@
         <v>15095</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -2105,7 +2403,7 @@
         <v>14915</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -2146,7 +2444,7 @@
         <v>14985</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -2187,7 +2485,7 @@
         <v>35430</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -2228,7 +2526,7 @@
         <v>9938</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2243,14 +2541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2258,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2266,7 +2564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2274,7 +2572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2580,7 @@
         <v>43913</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2290,7 +2588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2298,7 +2596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2306,7 +2604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2314,17 +2612,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2332,12 +2630,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2348,7 +2646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2359,7 +2657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2370,7 +2668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2381,7 +2679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2392,7 +2690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2403,7 +2701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2414,7 +2712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2425,7 +2723,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2436,7 +2734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2447,7 +2745,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2455,12 +2753,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2501,7 +2799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -2542,7 +2840,7 @@
         <v>11637</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -2583,7 +2881,7 @@
         <v>14287</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -2624,7 +2922,7 @@
         <v>35191</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -2665,7 +2963,7 @@
         <v>16075</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -2706,7 +3004,7 @@
         <v>16045</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -2747,7 +3045,7 @@
         <v>15762</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -2788,7 +3086,7 @@
         <v>33749</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -2829,7 +3127,7 @@
         <v>10428</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2844,16 +3142,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2861,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2869,7 +3167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2877,7 +3175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2885,7 +3183,7 @@
         <v>43913</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2893,7 +3191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2901,7 +3199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2909,7 +3207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2917,17 +3215,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2935,12 +3233,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2951,7 +3249,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2962,7 +3260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2973,7 +3271,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2984,7 +3282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2995,7 +3293,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -3006,7 +3304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3017,7 +3315,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3028,7 +3326,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -3039,7 +3337,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3050,7 +3348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3058,12 +3356,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -3104,7 +3402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -3145,7 +3443,7 @@
         <v>15256</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -3186,7 +3484,7 @@
         <v>18030</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -3227,7 +3525,7 @@
         <v>33913</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -3268,7 +3566,7 @@
         <v>20517</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -3309,7 +3607,7 @@
         <v>20226</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -3350,7 +3648,7 @@
         <v>20184</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -3391,7 +3689,7 @@
         <v>33639</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -3432,12 +3730,1821 @@
         <v>13590</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6D2DDC-9769-B74B-A7D7-3E3DDA4EDF12}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>113</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>16553</v>
+      </c>
+      <c r="C32">
+        <v>16822</v>
+      </c>
+      <c r="D32">
+        <v>16805</v>
+      </c>
+      <c r="E32">
+        <v>16750</v>
+      </c>
+      <c r="F32">
+        <v>16892</v>
+      </c>
+      <c r="G32">
+        <v>17110</v>
+      </c>
+      <c r="H32">
+        <v>16949</v>
+      </c>
+      <c r="I32">
+        <v>16956</v>
+      </c>
+      <c r="J32">
+        <v>16797</v>
+      </c>
+      <c r="K32">
+        <v>16796</v>
+      </c>
+      <c r="L32">
+        <v>16592</v>
+      </c>
+      <c r="M32">
+        <v>16383</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>21611</v>
+      </c>
+      <c r="C33">
+        <v>21146</v>
+      </c>
+      <c r="D33">
+        <v>21203</v>
+      </c>
+      <c r="E33">
+        <v>21319</v>
+      </c>
+      <c r="F33">
+        <v>21653</v>
+      </c>
+      <c r="G33">
+        <v>21489</v>
+      </c>
+      <c r="H33">
+        <v>21431</v>
+      </c>
+      <c r="I33">
+        <v>21890</v>
+      </c>
+      <c r="J33">
+        <v>21304</v>
+      </c>
+      <c r="K33">
+        <v>21820</v>
+      </c>
+      <c r="L33">
+        <v>21466</v>
+      </c>
+      <c r="M33">
+        <v>21252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>36701</v>
+      </c>
+      <c r="C34">
+        <v>38292</v>
+      </c>
+      <c r="D34">
+        <v>37758</v>
+      </c>
+      <c r="E34">
+        <v>36935</v>
+      </c>
+      <c r="F34">
+        <v>39280</v>
+      </c>
+      <c r="G34">
+        <v>38970</v>
+      </c>
+      <c r="H34">
+        <v>39379</v>
+      </c>
+      <c r="I34">
+        <v>39760</v>
+      </c>
+      <c r="J34">
+        <v>37507</v>
+      </c>
+      <c r="K34">
+        <v>37989</v>
+      </c>
+      <c r="L34">
+        <v>39055</v>
+      </c>
+      <c r="M34">
+        <v>37329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>35946</v>
+      </c>
+      <c r="C35">
+        <v>37207</v>
+      </c>
+      <c r="D35">
+        <v>37967</v>
+      </c>
+      <c r="E35">
+        <v>36908</v>
+      </c>
+      <c r="F35">
+        <v>35882</v>
+      </c>
+      <c r="G35">
+        <v>34207</v>
+      </c>
+      <c r="H35">
+        <v>28413</v>
+      </c>
+      <c r="I35">
+        <v>24317</v>
+      </c>
+      <c r="J35">
+        <v>21087</v>
+      </c>
+      <c r="K35">
+        <v>21328</v>
+      </c>
+      <c r="L35">
+        <v>22304</v>
+      </c>
+      <c r="M35">
+        <v>24685</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>37256</v>
+      </c>
+      <c r="C36">
+        <v>38170</v>
+      </c>
+      <c r="D36">
+        <v>36989</v>
+      </c>
+      <c r="E36">
+        <v>36312</v>
+      </c>
+      <c r="F36">
+        <v>35806</v>
+      </c>
+      <c r="G36">
+        <v>33673</v>
+      </c>
+      <c r="H36">
+        <v>29454</v>
+      </c>
+      <c r="I36">
+        <v>23925</v>
+      </c>
+      <c r="J36">
+        <v>20806</v>
+      </c>
+      <c r="K36">
+        <v>21240</v>
+      </c>
+      <c r="L36">
+        <v>22078</v>
+      </c>
+      <c r="M36">
+        <v>24735</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>35991</v>
+      </c>
+      <c r="C37">
+        <v>36555</v>
+      </c>
+      <c r="D37">
+        <v>36104</v>
+      </c>
+      <c r="E37">
+        <v>35666</v>
+      </c>
+      <c r="F37">
+        <v>34773</v>
+      </c>
+      <c r="G37">
+        <v>33224</v>
+      </c>
+      <c r="H37">
+        <v>28856</v>
+      </c>
+      <c r="I37">
+        <v>23206</v>
+      </c>
+      <c r="J37">
+        <v>20755</v>
+      </c>
+      <c r="K37">
+        <v>21108</v>
+      </c>
+      <c r="L37">
+        <v>22182</v>
+      </c>
+      <c r="M37">
+        <v>24730</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>35568</v>
+      </c>
+      <c r="C38">
+        <v>36688</v>
+      </c>
+      <c r="D38">
+        <v>37372</v>
+      </c>
+      <c r="E38">
+        <v>35760</v>
+      </c>
+      <c r="F38">
+        <v>38060</v>
+      </c>
+      <c r="G38">
+        <v>38227</v>
+      </c>
+      <c r="H38">
+        <v>38800</v>
+      </c>
+      <c r="I38">
+        <v>38172</v>
+      </c>
+      <c r="J38">
+        <v>38202</v>
+      </c>
+      <c r="K38">
+        <v>36091</v>
+      </c>
+      <c r="L38">
+        <v>37331</v>
+      </c>
+      <c r="M38">
+        <v>35759</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>15230</v>
+      </c>
+      <c r="C39">
+        <v>15507</v>
+      </c>
+      <c r="D39">
+        <v>15380</v>
+      </c>
+      <c r="E39">
+        <v>15658</v>
+      </c>
+      <c r="F39">
+        <v>15729</v>
+      </c>
+      <c r="G39">
+        <v>15977</v>
+      </c>
+      <c r="H39">
+        <v>15878</v>
+      </c>
+      <c r="I39">
+        <v>15758</v>
+      </c>
+      <c r="J39">
+        <v>15610</v>
+      </c>
+      <c r="K39">
+        <v>15594</v>
+      </c>
+      <c r="L39">
+        <v>15378</v>
+      </c>
+      <c r="M39">
+        <v>15514</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0A189A-7243-6E4D-9BB1-6FC418E826F7}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>98</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>5395</v>
+      </c>
+      <c r="C32">
+        <v>5590</v>
+      </c>
+      <c r="D32">
+        <v>5599</v>
+      </c>
+      <c r="E32">
+        <v>5653</v>
+      </c>
+      <c r="F32">
+        <v>5683</v>
+      </c>
+      <c r="G32">
+        <v>5740</v>
+      </c>
+      <c r="H32">
+        <v>5789</v>
+      </c>
+      <c r="I32">
+        <v>5755</v>
+      </c>
+      <c r="J32">
+        <v>5894</v>
+      </c>
+      <c r="K32">
+        <v>5697</v>
+      </c>
+      <c r="L32">
+        <v>5678</v>
+      </c>
+      <c r="M32">
+        <v>5498</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>7810</v>
+      </c>
+      <c r="C33">
+        <v>7807</v>
+      </c>
+      <c r="D33">
+        <v>7709</v>
+      </c>
+      <c r="E33">
+        <v>7791</v>
+      </c>
+      <c r="F33">
+        <v>8000</v>
+      </c>
+      <c r="G33">
+        <v>7861</v>
+      </c>
+      <c r="H33">
+        <v>7926</v>
+      </c>
+      <c r="I33">
+        <v>7824</v>
+      </c>
+      <c r="J33">
+        <v>7840</v>
+      </c>
+      <c r="K33">
+        <v>7750</v>
+      </c>
+      <c r="L33">
+        <v>7773</v>
+      </c>
+      <c r="M33">
+        <v>7757</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>34029</v>
+      </c>
+      <c r="C34">
+        <v>33225</v>
+      </c>
+      <c r="D34">
+        <v>33074</v>
+      </c>
+      <c r="E34">
+        <v>32546</v>
+      </c>
+      <c r="F34">
+        <v>33763</v>
+      </c>
+      <c r="G34">
+        <v>33215</v>
+      </c>
+      <c r="H34">
+        <v>34240</v>
+      </c>
+      <c r="I34">
+        <v>35200</v>
+      </c>
+      <c r="J34">
+        <v>32291</v>
+      </c>
+      <c r="K34">
+        <v>33869</v>
+      </c>
+      <c r="L34">
+        <v>34451</v>
+      </c>
+      <c r="M34">
+        <v>33126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>32709</v>
+      </c>
+      <c r="C35">
+        <v>34850</v>
+      </c>
+      <c r="D35">
+        <v>32771</v>
+      </c>
+      <c r="E35">
+        <v>33196</v>
+      </c>
+      <c r="F35">
+        <v>31518</v>
+      </c>
+      <c r="G35">
+        <v>31477</v>
+      </c>
+      <c r="H35">
+        <v>28380</v>
+      </c>
+      <c r="I35">
+        <v>21406</v>
+      </c>
+      <c r="J35">
+        <v>11495</v>
+      </c>
+      <c r="K35">
+        <v>8049</v>
+      </c>
+      <c r="L35">
+        <v>8049</v>
+      </c>
+      <c r="M35">
+        <v>8867</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>31715</v>
+      </c>
+      <c r="C36">
+        <v>32395</v>
+      </c>
+      <c r="D36">
+        <v>32433</v>
+      </c>
+      <c r="E36">
+        <v>33691</v>
+      </c>
+      <c r="F36">
+        <v>33890</v>
+      </c>
+      <c r="G36">
+        <v>31625</v>
+      </c>
+      <c r="H36">
+        <v>27445</v>
+      </c>
+      <c r="I36">
+        <v>20404</v>
+      </c>
+      <c r="J36">
+        <v>11874</v>
+      </c>
+      <c r="K36">
+        <v>8111</v>
+      </c>
+      <c r="L36">
+        <v>7896</v>
+      </c>
+      <c r="M36">
+        <v>8868</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>31743</v>
+      </c>
+      <c r="C37">
+        <v>32547</v>
+      </c>
+      <c r="D37">
+        <v>31394</v>
+      </c>
+      <c r="E37">
+        <v>31441</v>
+      </c>
+      <c r="F37">
+        <v>32182</v>
+      </c>
+      <c r="G37">
+        <v>30575</v>
+      </c>
+      <c r="H37">
+        <v>27285</v>
+      </c>
+      <c r="I37">
+        <v>20204</v>
+      </c>
+      <c r="J37">
+        <v>11524</v>
+      </c>
+      <c r="K37">
+        <v>7985</v>
+      </c>
+      <c r="L37">
+        <v>7893</v>
+      </c>
+      <c r="M37">
+        <v>8775</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>33452</v>
+      </c>
+      <c r="C38">
+        <v>32386</v>
+      </c>
+      <c r="D38">
+        <v>30464</v>
+      </c>
+      <c r="E38">
+        <v>31806</v>
+      </c>
+      <c r="F38">
+        <v>31393</v>
+      </c>
+      <c r="G38">
+        <v>31022</v>
+      </c>
+      <c r="H38">
+        <v>31617</v>
+      </c>
+      <c r="I38">
+        <v>30864</v>
+      </c>
+      <c r="J38">
+        <v>31893</v>
+      </c>
+      <c r="K38">
+        <v>31256</v>
+      </c>
+      <c r="L38">
+        <v>33825</v>
+      </c>
+      <c r="M38">
+        <v>30584</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>4923</v>
+      </c>
+      <c r="C39">
+        <v>4946</v>
+      </c>
+      <c r="D39">
+        <v>5035</v>
+      </c>
+      <c r="E39">
+        <v>4989</v>
+      </c>
+      <c r="F39">
+        <v>5030</v>
+      </c>
+      <c r="G39">
+        <v>5143</v>
+      </c>
+      <c r="H39">
+        <v>5044</v>
+      </c>
+      <c r="I39">
+        <v>5063</v>
+      </c>
+      <c r="J39">
+        <v>5086</v>
+      </c>
+      <c r="K39">
+        <v>5107</v>
+      </c>
+      <c r="L39">
+        <v>5082</v>
+      </c>
+      <c r="M39">
+        <v>5067</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7D43C4-403B-B64A-9441-72B8C64BA6AB}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>113</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>16037</v>
+      </c>
+      <c r="C32">
+        <v>16811</v>
+      </c>
+      <c r="D32">
+        <v>16802</v>
+      </c>
+      <c r="E32">
+        <v>17054</v>
+      </c>
+      <c r="F32">
+        <v>16958</v>
+      </c>
+      <c r="G32">
+        <v>17228</v>
+      </c>
+      <c r="H32">
+        <v>17509</v>
+      </c>
+      <c r="I32">
+        <v>17286</v>
+      </c>
+      <c r="J32">
+        <v>17529</v>
+      </c>
+      <c r="K32">
+        <v>16957</v>
+      </c>
+      <c r="L32">
+        <v>16674</v>
+      </c>
+      <c r="M32">
+        <v>16355</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>20320</v>
+      </c>
+      <c r="C33">
+        <v>20469</v>
+      </c>
+      <c r="D33">
+        <v>20385</v>
+      </c>
+      <c r="E33">
+        <v>20556</v>
+      </c>
+      <c r="F33">
+        <v>21235</v>
+      </c>
+      <c r="G33">
+        <v>20690</v>
+      </c>
+      <c r="H33">
+        <v>20729</v>
+      </c>
+      <c r="I33">
+        <v>20538</v>
+      </c>
+      <c r="J33">
+        <v>20501</v>
+      </c>
+      <c r="K33">
+        <v>20317</v>
+      </c>
+      <c r="L33">
+        <v>20192</v>
+      </c>
+      <c r="M33">
+        <v>20330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>39704</v>
+      </c>
+      <c r="C34">
+        <v>36770</v>
+      </c>
+      <c r="D34">
+        <v>38653</v>
+      </c>
+      <c r="E34">
+        <v>38305</v>
+      </c>
+      <c r="F34">
+        <v>38488</v>
+      </c>
+      <c r="G34">
+        <v>37907</v>
+      </c>
+      <c r="H34">
+        <v>40090</v>
+      </c>
+      <c r="I34">
+        <v>40170</v>
+      </c>
+      <c r="J34">
+        <v>38684</v>
+      </c>
+      <c r="K34">
+        <v>38930</v>
+      </c>
+      <c r="L34">
+        <v>38457</v>
+      </c>
+      <c r="M34">
+        <v>38783</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>39286</v>
+      </c>
+      <c r="C35">
+        <v>36968</v>
+      </c>
+      <c r="D35">
+        <v>37380</v>
+      </c>
+      <c r="E35">
+        <v>35809</v>
+      </c>
+      <c r="F35">
+        <v>35040</v>
+      </c>
+      <c r="G35">
+        <v>34644</v>
+      </c>
+      <c r="H35">
+        <v>30109</v>
+      </c>
+      <c r="I35">
+        <v>23613</v>
+      </c>
+      <c r="J35">
+        <v>20040</v>
+      </c>
+      <c r="K35">
+        <v>20257</v>
+      </c>
+      <c r="L35">
+        <v>21458</v>
+      </c>
+      <c r="M35">
+        <v>24027</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>34832</v>
+      </c>
+      <c r="C36">
+        <v>37521</v>
+      </c>
+      <c r="D36">
+        <v>36179</v>
+      </c>
+      <c r="E36">
+        <v>35779</v>
+      </c>
+      <c r="F36">
+        <v>34896</v>
+      </c>
+      <c r="G36">
+        <v>34207</v>
+      </c>
+      <c r="H36">
+        <v>28972</v>
+      </c>
+      <c r="I36">
+        <v>22224</v>
+      </c>
+      <c r="J36">
+        <v>19902</v>
+      </c>
+      <c r="K36">
+        <v>20286</v>
+      </c>
+      <c r="L36">
+        <v>21272</v>
+      </c>
+      <c r="M36">
+        <v>23918</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>37669</v>
+      </c>
+      <c r="C37">
+        <v>36798</v>
+      </c>
+      <c r="D37">
+        <v>35864</v>
+      </c>
+      <c r="E37">
+        <v>35284</v>
+      </c>
+      <c r="F37">
+        <v>36048</v>
+      </c>
+      <c r="G37">
+        <v>34489</v>
+      </c>
+      <c r="H37">
+        <v>29379</v>
+      </c>
+      <c r="I37">
+        <v>21871</v>
+      </c>
+      <c r="J37">
+        <v>19834</v>
+      </c>
+      <c r="K37">
+        <v>19902</v>
+      </c>
+      <c r="L37">
+        <v>21123</v>
+      </c>
+      <c r="M37">
+        <v>23529</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>37573</v>
+      </c>
+      <c r="C38">
+        <v>36425</v>
+      </c>
+      <c r="D38">
+        <v>36144</v>
+      </c>
+      <c r="E38">
+        <v>35498</v>
+      </c>
+      <c r="F38">
+        <v>35536</v>
+      </c>
+      <c r="G38">
+        <v>36252</v>
+      </c>
+      <c r="H38">
+        <v>36479</v>
+      </c>
+      <c r="I38">
+        <v>36677</v>
+      </c>
+      <c r="J38">
+        <v>35404</v>
+      </c>
+      <c r="K38">
+        <v>35551</v>
+      </c>
+      <c r="L38">
+        <v>38595</v>
+      </c>
+      <c r="M38">
+        <v>37466</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>14838</v>
+      </c>
+      <c r="C39">
+        <v>14936</v>
+      </c>
+      <c r="D39">
+        <v>15211</v>
+      </c>
+      <c r="E39">
+        <v>15273</v>
+      </c>
+      <c r="F39">
+        <v>15369</v>
+      </c>
+      <c r="G39">
+        <v>15506</v>
+      </c>
+      <c r="H39">
+        <v>15470</v>
+      </c>
+      <c r="I39">
+        <v>15419</v>
+      </c>
+      <c r="J39">
+        <v>15187</v>
+      </c>
+      <c r="K39">
+        <v>15295</v>
+      </c>
+      <c r="L39">
+        <v>15333</v>
+      </c>
+      <c r="M39">
+        <v>15319</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add K189D / K189N neuts
</commit_message>
<xml_diff>
--- a/data/neut_plate_reader_data/HC060002.xlsx
+++ b/data/neut_plate_reader_data/HC060002.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/fh/fast/bloom_j/computational_notebooks/reguia/2020/validation/data/neut_plate_reader_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/bloom_j/computational_notebooks/reguia/2020/validation/data/neut_plate_reader_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B13E22-864F-7647-A8AE-0428773DD993}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D39DA95-1A4C-E943-A0E9-66E243B075BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="21100" windowHeight="14860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="21100" windowHeight="14860" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F193D" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="I192E" sheetId="6" r:id="rId5"/>
     <sheet name="F159G" sheetId="7" r:id="rId6"/>
     <sheet name="WT2" sheetId="8" r:id="rId7"/>
+    <sheet name="May K189D" sheetId="9" r:id="rId8"/>
+    <sheet name="May K189N" sheetId="10" r:id="rId9"/>
+    <sheet name="May WT" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -102,6 +105,97 @@
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -662,8 +756,190 @@
 </comments>
 </file>
 
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="83">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -879,13 +1155,46 @@
   </si>
   <si>
     <t>9:36:25 AM</t>
+  </si>
+  <si>
+    <t>5/9/2020 9:09:28 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 24.2 °C</t>
+  </si>
+  <si>
+    <t>5/9/2020 9:08:31 AM</t>
+  </si>
+  <si>
+    <t>9:07:33 AM</t>
+  </si>
+  <si>
+    <t>5/9/2020 9:07:11 AM</t>
+  </si>
+  <si>
+    <t>5/9/2020 9:06:13 AM</t>
+  </si>
+  <si>
+    <t>9:05:13 AM</t>
+  </si>
+  <si>
+    <t>5/9/2020 9:04:56 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 24.1 °C</t>
+  </si>
+  <si>
+    <t>5/9/2020 9:03:59 AM</t>
+  </si>
+  <si>
+    <t>9:03:01 AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,6 +1222,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1939,6 +2255,607 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D957750B-53D9-864C-BE17-89F55030ACD8}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>111</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>15182</v>
+      </c>
+      <c r="C32">
+        <v>14882</v>
+      </c>
+      <c r="D32">
+        <v>15061</v>
+      </c>
+      <c r="E32">
+        <v>15409</v>
+      </c>
+      <c r="F32">
+        <v>15417</v>
+      </c>
+      <c r="G32">
+        <v>16208</v>
+      </c>
+      <c r="H32">
+        <v>15764</v>
+      </c>
+      <c r="I32">
+        <v>15548</v>
+      </c>
+      <c r="J32">
+        <v>15445</v>
+      </c>
+      <c r="K32">
+        <v>15782</v>
+      </c>
+      <c r="L32">
+        <v>15433</v>
+      </c>
+      <c r="M32">
+        <v>15257</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>18282</v>
+      </c>
+      <c r="C33">
+        <v>18186</v>
+      </c>
+      <c r="D33">
+        <v>18231</v>
+      </c>
+      <c r="E33">
+        <v>18290</v>
+      </c>
+      <c r="F33">
+        <v>18510</v>
+      </c>
+      <c r="G33">
+        <v>18463</v>
+      </c>
+      <c r="H33">
+        <v>18372</v>
+      </c>
+      <c r="I33">
+        <v>18682</v>
+      </c>
+      <c r="J33">
+        <v>18557</v>
+      </c>
+      <c r="K33">
+        <v>18424</v>
+      </c>
+      <c r="L33">
+        <v>18316</v>
+      </c>
+      <c r="M33">
+        <v>19002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>41595</v>
+      </c>
+      <c r="C34">
+        <v>40944</v>
+      </c>
+      <c r="D34">
+        <v>39931</v>
+      </c>
+      <c r="E34">
+        <v>42953</v>
+      </c>
+      <c r="F34">
+        <v>43062</v>
+      </c>
+      <c r="G34">
+        <v>42755</v>
+      </c>
+      <c r="H34">
+        <v>41824</v>
+      </c>
+      <c r="I34">
+        <v>42312</v>
+      </c>
+      <c r="J34">
+        <v>41418</v>
+      </c>
+      <c r="K34">
+        <v>41888</v>
+      </c>
+      <c r="L34">
+        <v>41772</v>
+      </c>
+      <c r="M34">
+        <v>40485</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>40395</v>
+      </c>
+      <c r="C35">
+        <v>39906</v>
+      </c>
+      <c r="D35">
+        <v>39555</v>
+      </c>
+      <c r="E35">
+        <v>39557</v>
+      </c>
+      <c r="F35">
+        <v>38741</v>
+      </c>
+      <c r="G35">
+        <v>36701</v>
+      </c>
+      <c r="H35">
+        <v>31705</v>
+      </c>
+      <c r="I35">
+        <v>23240</v>
+      </c>
+      <c r="J35">
+        <v>18768</v>
+      </c>
+      <c r="K35">
+        <v>18929</v>
+      </c>
+      <c r="L35">
+        <v>19735</v>
+      </c>
+      <c r="M35">
+        <v>22195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>39420</v>
+      </c>
+      <c r="C36">
+        <v>40717</v>
+      </c>
+      <c r="D36">
+        <v>38071</v>
+      </c>
+      <c r="E36">
+        <v>40115</v>
+      </c>
+      <c r="F36">
+        <v>38672</v>
+      </c>
+      <c r="G36">
+        <v>35918</v>
+      </c>
+      <c r="H36">
+        <v>30089</v>
+      </c>
+      <c r="I36">
+        <v>22363</v>
+      </c>
+      <c r="J36">
+        <v>18486</v>
+      </c>
+      <c r="K36">
+        <v>18438</v>
+      </c>
+      <c r="L36">
+        <v>19765</v>
+      </c>
+      <c r="M36">
+        <v>22172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>38895</v>
+      </c>
+      <c r="C37">
+        <v>38689</v>
+      </c>
+      <c r="D37">
+        <v>35792</v>
+      </c>
+      <c r="E37">
+        <v>38422</v>
+      </c>
+      <c r="F37">
+        <v>37305</v>
+      </c>
+      <c r="G37">
+        <v>35814</v>
+      </c>
+      <c r="H37">
+        <v>29944</v>
+      </c>
+      <c r="I37">
+        <v>22712</v>
+      </c>
+      <c r="J37">
+        <v>18426</v>
+      </c>
+      <c r="K37">
+        <v>18453</v>
+      </c>
+      <c r="L37">
+        <v>19865</v>
+      </c>
+      <c r="M37">
+        <v>22255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>39760</v>
+      </c>
+      <c r="C38">
+        <v>40075</v>
+      </c>
+      <c r="D38">
+        <v>39305</v>
+      </c>
+      <c r="E38">
+        <v>39121</v>
+      </c>
+      <c r="F38">
+        <v>39044</v>
+      </c>
+      <c r="G38">
+        <v>38343</v>
+      </c>
+      <c r="H38">
+        <v>40431</v>
+      </c>
+      <c r="I38">
+        <v>41611</v>
+      </c>
+      <c r="J38">
+        <v>40273</v>
+      </c>
+      <c r="K38">
+        <v>40910</v>
+      </c>
+      <c r="L38">
+        <v>39536</v>
+      </c>
+      <c r="M38">
+        <v>39962</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>13895</v>
+      </c>
+      <c r="C39">
+        <v>14069</v>
+      </c>
+      <c r="D39">
+        <v>14168</v>
+      </c>
+      <c r="E39">
+        <v>14537</v>
+      </c>
+      <c r="F39">
+        <v>14466</v>
+      </c>
+      <c r="G39">
+        <v>14641</v>
+      </c>
+      <c r="H39">
+        <v>14704</v>
+      </c>
+      <c r="I39">
+        <v>14633</v>
+      </c>
+      <c r="J39">
+        <v>14761</v>
+      </c>
+      <c r="K39">
+        <v>14741</v>
+      </c>
+      <c r="L39">
+        <v>14585</v>
+      </c>
+      <c r="M39">
+        <v>14693</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M43"/>
@@ -3748,7 +4665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6D2DDC-9769-B74B-A7D7-3E3DDA4EDF12}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -5551,4 +6468,1206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029F8E05-FFFE-7C4E-9E0D-F3983F4DC8F1}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>105</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>9919</v>
+      </c>
+      <c r="C32">
+        <v>10045</v>
+      </c>
+      <c r="D32">
+        <v>10081</v>
+      </c>
+      <c r="E32">
+        <v>10069</v>
+      </c>
+      <c r="F32">
+        <v>10020</v>
+      </c>
+      <c r="G32">
+        <v>10178</v>
+      </c>
+      <c r="H32">
+        <v>10174</v>
+      </c>
+      <c r="I32">
+        <v>10145</v>
+      </c>
+      <c r="J32">
+        <v>9998</v>
+      </c>
+      <c r="K32">
+        <v>10041</v>
+      </c>
+      <c r="L32">
+        <v>9998</v>
+      </c>
+      <c r="M32">
+        <v>9889</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>12698</v>
+      </c>
+      <c r="C33">
+        <v>12453</v>
+      </c>
+      <c r="D33">
+        <v>12287</v>
+      </c>
+      <c r="E33">
+        <v>12444</v>
+      </c>
+      <c r="F33">
+        <v>12612</v>
+      </c>
+      <c r="G33">
+        <v>12431</v>
+      </c>
+      <c r="H33">
+        <v>12439</v>
+      </c>
+      <c r="I33">
+        <v>12786</v>
+      </c>
+      <c r="J33">
+        <v>12356</v>
+      </c>
+      <c r="K33">
+        <v>12672</v>
+      </c>
+      <c r="L33">
+        <v>12563</v>
+      </c>
+      <c r="M33">
+        <v>12425</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>38497</v>
+      </c>
+      <c r="C34">
+        <v>41246</v>
+      </c>
+      <c r="D34">
+        <v>40915</v>
+      </c>
+      <c r="E34">
+        <v>39858</v>
+      </c>
+      <c r="F34">
+        <v>39548</v>
+      </c>
+      <c r="G34">
+        <v>39561</v>
+      </c>
+      <c r="H34">
+        <v>40712</v>
+      </c>
+      <c r="I34">
+        <v>40660</v>
+      </c>
+      <c r="J34">
+        <v>42209</v>
+      </c>
+      <c r="K34">
+        <v>39805</v>
+      </c>
+      <c r="L34">
+        <v>40148</v>
+      </c>
+      <c r="M34">
+        <v>39643</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>40001</v>
+      </c>
+      <c r="C35">
+        <v>40281</v>
+      </c>
+      <c r="D35">
+        <v>40057</v>
+      </c>
+      <c r="E35">
+        <v>39741</v>
+      </c>
+      <c r="F35">
+        <v>38218</v>
+      </c>
+      <c r="G35">
+        <v>38440</v>
+      </c>
+      <c r="H35">
+        <v>36142</v>
+      </c>
+      <c r="I35">
+        <v>32227</v>
+      </c>
+      <c r="J35">
+        <v>24022</v>
+      </c>
+      <c r="K35">
+        <v>16078</v>
+      </c>
+      <c r="L35">
+        <v>13544</v>
+      </c>
+      <c r="M35">
+        <v>14701</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>37575</v>
+      </c>
+      <c r="C36">
+        <v>39309</v>
+      </c>
+      <c r="D36">
+        <v>39273</v>
+      </c>
+      <c r="E36">
+        <v>38480</v>
+      </c>
+      <c r="F36">
+        <v>39847</v>
+      </c>
+      <c r="G36">
+        <v>38891</v>
+      </c>
+      <c r="H36">
+        <v>34873</v>
+      </c>
+      <c r="I36">
+        <v>30466</v>
+      </c>
+      <c r="J36">
+        <v>23911</v>
+      </c>
+      <c r="K36">
+        <v>15957</v>
+      </c>
+      <c r="L36">
+        <v>13382</v>
+      </c>
+      <c r="M36">
+        <v>14795</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>37129</v>
+      </c>
+      <c r="C37">
+        <v>40092</v>
+      </c>
+      <c r="D37">
+        <v>39149</v>
+      </c>
+      <c r="E37">
+        <v>37979</v>
+      </c>
+      <c r="F37">
+        <v>38133</v>
+      </c>
+      <c r="G37">
+        <v>38022</v>
+      </c>
+      <c r="H37">
+        <v>34725</v>
+      </c>
+      <c r="I37">
+        <v>31439</v>
+      </c>
+      <c r="J37">
+        <v>23069</v>
+      </c>
+      <c r="K37">
+        <v>15935</v>
+      </c>
+      <c r="L37">
+        <v>13485</v>
+      </c>
+      <c r="M37">
+        <v>14877</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>38017</v>
+      </c>
+      <c r="C38">
+        <v>39486</v>
+      </c>
+      <c r="D38">
+        <v>38839</v>
+      </c>
+      <c r="E38">
+        <v>38308</v>
+      </c>
+      <c r="F38">
+        <v>40097</v>
+      </c>
+      <c r="G38">
+        <v>39466</v>
+      </c>
+      <c r="H38">
+        <v>39417</v>
+      </c>
+      <c r="I38">
+        <v>39938</v>
+      </c>
+      <c r="J38">
+        <v>40532</v>
+      </c>
+      <c r="K38">
+        <v>40168</v>
+      </c>
+      <c r="L38">
+        <v>40954</v>
+      </c>
+      <c r="M38">
+        <v>37744</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>9276</v>
+      </c>
+      <c r="C39">
+        <v>9486</v>
+      </c>
+      <c r="D39">
+        <v>9514</v>
+      </c>
+      <c r="E39">
+        <v>9620</v>
+      </c>
+      <c r="F39">
+        <v>9707</v>
+      </c>
+      <c r="G39">
+        <v>9684</v>
+      </c>
+      <c r="H39">
+        <v>9664</v>
+      </c>
+      <c r="I39">
+        <v>9605</v>
+      </c>
+      <c r="J39">
+        <v>9595</v>
+      </c>
+      <c r="K39">
+        <v>9550</v>
+      </c>
+      <c r="L39">
+        <v>9511</v>
+      </c>
+      <c r="M39">
+        <v>9558</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB04F96-1B10-BD42-8AA9-AA6552BAC465}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>115</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>19403</v>
+      </c>
+      <c r="C32">
+        <v>19685</v>
+      </c>
+      <c r="D32">
+        <v>19526</v>
+      </c>
+      <c r="E32">
+        <v>19748</v>
+      </c>
+      <c r="F32">
+        <v>19870</v>
+      </c>
+      <c r="G32">
+        <v>19691</v>
+      </c>
+      <c r="H32">
+        <v>19575</v>
+      </c>
+      <c r="I32">
+        <v>19717</v>
+      </c>
+      <c r="J32">
+        <v>19285</v>
+      </c>
+      <c r="K32">
+        <v>19152</v>
+      </c>
+      <c r="L32">
+        <v>18939</v>
+      </c>
+      <c r="M32">
+        <v>18369</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>24851</v>
+      </c>
+      <c r="C33">
+        <v>24149</v>
+      </c>
+      <c r="D33">
+        <v>24293</v>
+      </c>
+      <c r="E33">
+        <v>24444</v>
+      </c>
+      <c r="F33">
+        <v>24687</v>
+      </c>
+      <c r="G33">
+        <v>24718</v>
+      </c>
+      <c r="H33">
+        <v>24605</v>
+      </c>
+      <c r="I33">
+        <v>24969</v>
+      </c>
+      <c r="J33">
+        <v>24086</v>
+      </c>
+      <c r="K33">
+        <v>24931</v>
+      </c>
+      <c r="L33">
+        <v>24639</v>
+      </c>
+      <c r="M33">
+        <v>24230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>36363</v>
+      </c>
+      <c r="C34">
+        <v>37581</v>
+      </c>
+      <c r="D34">
+        <v>36785</v>
+      </c>
+      <c r="E34">
+        <v>37383</v>
+      </c>
+      <c r="F34">
+        <v>35880</v>
+      </c>
+      <c r="G34">
+        <v>36607</v>
+      </c>
+      <c r="H34">
+        <v>38908</v>
+      </c>
+      <c r="I34">
+        <v>37607</v>
+      </c>
+      <c r="J34">
+        <v>36560</v>
+      </c>
+      <c r="K34">
+        <v>37062</v>
+      </c>
+      <c r="L34">
+        <v>36822</v>
+      </c>
+      <c r="M34">
+        <v>38217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>36106</v>
+      </c>
+      <c r="C35">
+        <v>35741</v>
+      </c>
+      <c r="D35">
+        <v>35915</v>
+      </c>
+      <c r="E35">
+        <v>36096</v>
+      </c>
+      <c r="F35">
+        <v>34882</v>
+      </c>
+      <c r="G35">
+        <v>35474</v>
+      </c>
+      <c r="H35">
+        <v>34016</v>
+      </c>
+      <c r="I35">
+        <v>32294</v>
+      </c>
+      <c r="J35">
+        <v>27876</v>
+      </c>
+      <c r="K35">
+        <v>25095</v>
+      </c>
+      <c r="L35">
+        <v>25869</v>
+      </c>
+      <c r="M35">
+        <v>28769</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>35538</v>
+      </c>
+      <c r="C36">
+        <v>36327</v>
+      </c>
+      <c r="D36">
+        <v>36933</v>
+      </c>
+      <c r="E36">
+        <v>36284</v>
+      </c>
+      <c r="F36">
+        <v>35874</v>
+      </c>
+      <c r="G36">
+        <v>35642</v>
+      </c>
+      <c r="H36">
+        <v>33186</v>
+      </c>
+      <c r="I36">
+        <v>31585</v>
+      </c>
+      <c r="J36">
+        <v>27419</v>
+      </c>
+      <c r="K36">
+        <v>25209</v>
+      </c>
+      <c r="L36">
+        <v>26095</v>
+      </c>
+      <c r="M36">
+        <v>28607</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>36202</v>
+      </c>
+      <c r="C37">
+        <v>35924</v>
+      </c>
+      <c r="D37">
+        <v>35738</v>
+      </c>
+      <c r="E37">
+        <v>35469</v>
+      </c>
+      <c r="F37">
+        <v>36278</v>
+      </c>
+      <c r="G37">
+        <v>34698</v>
+      </c>
+      <c r="H37">
+        <v>33935</v>
+      </c>
+      <c r="I37">
+        <v>31703</v>
+      </c>
+      <c r="J37">
+        <v>27617</v>
+      </c>
+      <c r="K37">
+        <v>24915</v>
+      </c>
+      <c r="L37">
+        <v>26016</v>
+      </c>
+      <c r="M37">
+        <v>28648</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>35991</v>
+      </c>
+      <c r="C38">
+        <v>35700</v>
+      </c>
+      <c r="D38">
+        <v>35302</v>
+      </c>
+      <c r="E38">
+        <v>35211</v>
+      </c>
+      <c r="F38">
+        <v>35559</v>
+      </c>
+      <c r="G38">
+        <v>36262</v>
+      </c>
+      <c r="H38">
+        <v>36594</v>
+      </c>
+      <c r="I38">
+        <v>35803</v>
+      </c>
+      <c r="J38">
+        <v>36565</v>
+      </c>
+      <c r="K38">
+        <v>35070</v>
+      </c>
+      <c r="L38">
+        <v>36517</v>
+      </c>
+      <c r="M38">
+        <v>35362</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>17655</v>
+      </c>
+      <c r="C39">
+        <v>18147</v>
+      </c>
+      <c r="D39">
+        <v>18165</v>
+      </c>
+      <c r="E39">
+        <v>18321</v>
+      </c>
+      <c r="F39">
+        <v>18529</v>
+      </c>
+      <c r="G39">
+        <v>18926</v>
+      </c>
+      <c r="H39">
+        <v>18736</v>
+      </c>
+      <c r="I39">
+        <v>18829</v>
+      </c>
+      <c r="J39">
+        <v>18555</v>
+      </c>
+      <c r="K39">
+        <v>18554</v>
+      </c>
+      <c r="L39">
+        <v>18594</v>
+      </c>
+      <c r="M39">
+        <v>18677</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>